<commit_message>
fixed door directions in xcel sheet
</commit_message>
<xml_diff>
--- a/ClueBoard.xlsx
+++ b/ClueBoard.xlsx
@@ -54,34 +54,34 @@
     <t>CD</t>
   </si>
   <si>
-    <t>LD</t>
-  </si>
-  <si>
-    <t>GD</t>
-  </si>
-  <si>
-    <t>TD</t>
-  </si>
-  <si>
     <t>KD</t>
   </si>
   <si>
     <t>SD</t>
   </si>
   <si>
-    <t>RD</t>
+    <t>W</t>
   </si>
   <si>
-    <t>BD</t>
+    <t>QR</t>
   </si>
   <si>
-    <t>DD</t>
+    <t>LL</t>
   </si>
   <si>
-    <t>QD</t>
+    <t>TL</t>
   </si>
   <si>
-    <t>W</t>
+    <t>GU</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>BU</t>
+  </si>
+  <si>
+    <t>DL</t>
   </si>
 </sst>
 </file>
@@ -459,7 +459,7 @@
   <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,10 +478,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -526,10 +526,10 @@
         <v>2</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>1</v>
@@ -549,10 +549,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>2</v>
@@ -597,10 +597,10 @@
         <v>2</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>11</v>
@@ -620,10 +620,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>2</v>
@@ -668,10 +668,10 @@
         <v>2</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>1</v>
@@ -691,10 +691,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>2</v>
@@ -739,16 +739,16 @@
         <v>2</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
@@ -762,10 +762,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>2</v>
@@ -780,19 +780,19 @@
         <v>2</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>2</v>
@@ -810,16 +810,16 @@
         <v>2</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="W5" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
@@ -833,58 +833,58 @@
         <v>3</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>4</v>
@@ -904,58 +904,58 @@
         <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V7" s="2" t="s">
         <v>4</v>
@@ -975,7 +975,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
@@ -990,7 +990,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>0</v>
@@ -1014,10 +1014,10 @@
         <v>0</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>4</v>
@@ -1040,13 +1040,13 @@
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
@@ -1061,7 +1061,7 @@
         <v>9</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>0</v>
@@ -1085,10 +1085,10 @@
         <v>0</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S9" s="2" t="s">
         <v>4</v>
@@ -1108,16 +1108,16 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
@@ -1129,10 +1129,10 @@
         <v>9</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>0</v>
@@ -1156,13 +1156,13 @@
         <v>0</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="T10" s="2" t="s">
         <v>4</v>
@@ -1179,16 +1179,16 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
@@ -1203,7 +1203,7 @@
         <v>9</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>0</v>
@@ -1227,13 +1227,13 @@
         <v>0</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="T11" s="2" t="s">
         <v>4</v>
@@ -1250,16 +1250,16 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
@@ -1274,7 +1274,7 @@
         <v>9</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>0</v>
@@ -1298,13 +1298,13 @@
         <v>0</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="T12" s="2" t="s">
         <v>4</v>
@@ -1321,58 +1321,58 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S13" s="2" t="s">
         <v>4</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
@@ -1422,10 +1422,10 @@
         <v>6</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>8</v>
@@ -1443,7 +1443,7 @@
         <v>8</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S14" s="2" t="s">
         <v>4</v>
@@ -1463,13 +1463,13 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>6</v>
@@ -1493,10 +1493,10 @@
         <v>6</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M15" s="3" t="s">
         <v>8</v>
@@ -1514,7 +1514,7 @@
         <v>8</v>
       </c>
       <c r="R15" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>4</v>
@@ -1534,17 +1534,17 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="E16" s="2" t="s">
         <v>6</v>
       </c>
@@ -1564,13 +1564,13 @@
         <v>6</v>
       </c>
       <c r="K16" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="N16" s="3" t="s">
         <v>8</v>
@@ -1585,7 +1585,7 @@
         <v>8</v>
       </c>
       <c r="R16" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S16" s="2" t="s">
         <v>4</v>
@@ -1605,17 +1605,17 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="E17" s="2" t="s">
         <v>6</v>
       </c>
@@ -1635,13 +1635,13 @@
         <v>6</v>
       </c>
       <c r="K17" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="N17" s="3" t="s">
         <v>8</v>
@@ -1656,16 +1656,16 @@
         <v>8</v>
       </c>
       <c r="R17" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U17" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V17" s="2" t="s">
         <v>4</v>
@@ -1676,13 +1676,13 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>
@@ -1706,10 +1706,10 @@
         <v>6</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M18" s="3" t="s">
         <v>8</v>
@@ -1733,10 +1733,10 @@
         <v>8</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U18" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V18" s="2" t="s">
         <v>4</v>
@@ -1753,7 +1753,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -1777,43 +1777,43 @@
         <v>6</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="P19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="U19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="V19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="W19" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -1824,40 +1824,40 @@
         <v>5</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>7</v>
@@ -1866,7 +1866,7 @@
         <v>7</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>7</v>
@@ -1895,16 +1895,16 @@
         <v>5</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>10</v>
@@ -1916,7 +1916,7 @@
         <v>10</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>10</v>
@@ -1925,10 +1925,10 @@
         <v>10</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>7</v>
@@ -1972,10 +1972,10 @@
         <v>5</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>10</v>
@@ -1999,7 +1999,7 @@
         <v>10</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O22" s="2" t="s">
         <v>7</v>
@@ -2043,10 +2043,10 @@
         <v>5</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>10</v>
@@ -2067,10 +2067,10 @@
         <v>10</v>
       </c>
       <c r="M23" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="N23" s="6" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="O23" s="2" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
started project skeleton. Finished through BoardCell class
</commit_message>
<xml_diff>
--- a/ClueBoard.xlsx
+++ b/ClueBoard.xlsx
@@ -51,9 +51,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>CD</t>
-  </si>
-  <si>
     <t>KD</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>DL</t>
+  </si>
+  <si>
+    <t>CL</t>
   </si>
 </sst>
 </file>
@@ -456,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y29" sqref="Y29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,7 +467,7 @@
     <col min="1" max="24" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -478,10 +478,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
@@ -526,10 +526,10 @@
         <v>2</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U1" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>1</v>
@@ -537,8 +537,11 @@
       <c r="W1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="X1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -549,10 +552,10 @@
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>2</v>
@@ -597,19 +600,23 @@
         <v>2</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="X2">
+        <f>X1+1</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -620,10 +627,10 @@
         <v>3</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>2</v>
@@ -668,10 +675,10 @@
         <v>2</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>1</v>
@@ -679,8 +686,12 @@
       <c r="W3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X23" si="0">X2+1</f>
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -691,10 +702,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>2</v>
@@ -739,19 +750,23 @@
         <v>2</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -762,10 +777,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>2</v>
@@ -780,19 +795,19 @@
         <v>2</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>2</v>
@@ -810,19 +825,23 @@
         <v>2</v>
       </c>
       <c r="T5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -833,58 +852,58 @@
         <v>3</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V6" s="2" t="s">
         <v>4</v>
@@ -892,8 +911,12 @@
       <c r="W6" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="X6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -904,58 +927,58 @@
         <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V7" s="2" t="s">
         <v>4</v>
@@ -963,8 +986,12 @@
       <c r="W7" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="X7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -975,7 +1002,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
@@ -990,7 +1017,7 @@
         <v>9</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>0</v>
@@ -1014,10 +1041,10 @@
         <v>0</v>
       </c>
       <c r="Q8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S8" s="2" t="s">
         <v>4</v>
@@ -1034,19 +1061,23 @@
       <c r="W8" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="X8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
@@ -1061,7 +1092,7 @@
         <v>9</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>0</v>
@@ -1085,10 +1116,10 @@
         <v>0</v>
       </c>
       <c r="Q9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S9" s="2" t="s">
         <v>4</v>
@@ -1105,19 +1136,23 @@
       <c r="W9" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="X9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
@@ -1129,41 +1164,41 @@
         <v>9</v>
       </c>
       <c r="H10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="R10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S10" s="4" t="s">
-        <v>16</v>
-      </c>
       <c r="T10" s="2" t="s">
         <v>4</v>
       </c>
@@ -1176,19 +1211,23 @@
       <c r="W10" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="X10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
@@ -1203,7 +1242,7 @@
         <v>9</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>0</v>
@@ -1227,13 +1266,13 @@
         <v>0</v>
       </c>
       <c r="Q11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T11" s="2" t="s">
         <v>4</v>
@@ -1247,19 +1286,23 @@
       <c r="W11" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="X11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
@@ -1274,478 +1317,506 @@
         <v>9</v>
       </c>
       <c r="I12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="T12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="J12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="R12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S12" s="4" t="s">
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="T12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="W12" s="2" t="s">
-        <v>4</v>
+      <c r="N16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="V16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="R13" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="W13" s="2" t="s">
-        <v>4</v>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="U17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="W14" s="2" t="s">
-        <v>4</v>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="U18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="W15" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="V16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="W16" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="T17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="U17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="V17" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="W17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="S18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="T18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="U18" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="V18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="W18" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
@@ -1753,7 +1824,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>6</v>
@@ -1777,46 +1848,50 @@
         <v>6</v>
       </c>
       <c r="K19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W19" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1824,40 +1899,40 @@
         <v>5</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N20" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O20" s="2" t="s">
         <v>7</v>
@@ -1866,7 +1941,7 @@
         <v>7</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="R20" s="2" t="s">
         <v>7</v>
@@ -1886,8 +1961,12 @@
       <c r="W20" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="X20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
@@ -1895,16 +1974,16 @@
         <v>5</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>10</v>
@@ -1916,7 +1995,7 @@
         <v>10</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K21" s="2" t="s">
         <v>10</v>
@@ -1925,10 +2004,10 @@
         <v>10</v>
       </c>
       <c r="M21" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="N21" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O21" s="2" t="s">
         <v>7</v>
@@ -1957,8 +2036,12 @@
       <c r="W21" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="X21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1972,10 +2055,10 @@
         <v>5</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>10</v>
@@ -1999,7 +2082,7 @@
         <v>10</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O22" s="2" t="s">
         <v>7</v>
@@ -2028,8 +2111,12 @@
       <c r="W22" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="X22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
@@ -2043,10 +2130,10 @@
         <v>5</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>10</v>
@@ -2067,37 +2154,134 @@
         <v>10</v>
       </c>
       <c r="M23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="T23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="W23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <f>A24+1</f>
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:W24" si="1">B24+1</f>
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="N24">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="N23" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="O23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="T23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="V23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="W23" s="2" t="s">
-        <v>7</v>
+      <c r="P24">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="S24">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="U24">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="V24">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="W24">
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
'finished' skeleton for clueGame package
</commit_message>
<xml_diff>
--- a/ClueBoard.xlsx
+++ b/ClueBoard.xlsx
@@ -7,9 +7,7 @@
     <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="ClueBoard" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -459,7 +457,7 @@
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y29" sqref="Y29"/>
+      <selection activeCell="Y11" sqref="Y11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2288,28 +2286,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>